<commit_message>
Updated BT encounter summaries
</commit_message>
<xml_diff>
--- a/data/encounters/suspected_mortality_updated.xlsx
+++ b/data/encounters/suspected_mortality_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcusMichelangeli\GIT projects\Git_repo\drugged_lakes_griffith_repo\drugged_lakes\data\encounters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3058D5F2-AA8B-4FB6-A9BB-7BE8317C866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B4F44D-42AB-472F-9A9C-83E1C53231FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1275" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="90">
   <si>
     <t>individual_ID</t>
   </si>
@@ -163,9 +163,6 @@
     <t>likely_predated</t>
   </si>
   <si>
-    <t>alive_but_not_captured</t>
-  </si>
-  <si>
     <t>mortality</t>
   </si>
   <si>
@@ -293,13 +290,16 @@
   </si>
   <si>
     <t>did not move much</t>
+  </si>
+  <si>
+    <t>mortality?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -360,6 +360,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -402,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,6 +427,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,15 +728,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y17" sqref="Y17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.7109375" customWidth="1"/>
     <col min="6" max="7" width="24" bestFit="1" customWidth="1"/>
@@ -777,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>5</v>
@@ -786,28 +799,28 @@
         <v>6</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="S1" t="s">
-        <v>86</v>
-      </c>
       <c r="T1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>7</v>
@@ -816,27 +829,27 @@
         <v>8</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:27">
       <c r="A2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>25</v>
@@ -857,7 +870,7 @@
         <v>44833</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2">
         <v>0.2968805743704</v>
@@ -866,7 +879,7 @@
         <v>44835</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P2" s="1"/>
       <c r="R2" s="1"/>
@@ -887,15 +900,15 @@
         <v>38</v>
       </c>
       <c r="AA2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>10</v>
@@ -916,7 +929,7 @@
         <v>44838</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J3">
         <v>0.246416098381885</v>
@@ -925,7 +938,7 @@
         <v>44832</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -956,7 +969,7 @@
         <v>25</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X3" s="6">
         <v>44834</v>
@@ -965,15 +978,15 @@
         <v>44834</v>
       </c>
       <c r="Z3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>25</v>
@@ -994,7 +1007,7 @@
         <v>44829</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4">
         <v>0.20670888790561101</v>
@@ -1003,7 +1016,7 @@
         <v>44829</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1034,7 +1047,7 @@
         <v>22</v>
       </c>
       <c r="W4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X4" s="6">
         <v>44842</v>
@@ -1043,15 +1056,15 @@
         <v>44842</v>
       </c>
       <c r="Z4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>10</v>
@@ -1072,7 +1085,7 @@
         <v>44831</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J5">
         <v>0.36142689248335602</v>
@@ -1081,7 +1094,7 @@
         <v>44829</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -1112,7 +1125,7 @@
         <v>29</v>
       </c>
       <c r="W5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X5" s="6">
         <v>44832</v>
@@ -1121,15 +1134,15 @@
         <v>44832</v>
       </c>
       <c r="Z5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>25</v>
@@ -1150,7 +1163,7 @@
         <v>44847</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J6">
         <v>0.32346077598522799</v>
@@ -1159,7 +1172,7 @@
         <v>44847</v>
       </c>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P6" s="1"/>
       <c r="R6" s="1"/>
@@ -1182,10 +1195,10 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>25</v>
@@ -1206,7 +1219,7 @@
         <v>44858</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7">
         <v>0.11918318382607999</v>
@@ -1215,7 +1228,7 @@
         <v>44863</v>
       </c>
       <c r="L7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M7">
         <v>12</v>
@@ -1260,10 +1273,10 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>25</v>
@@ -1284,7 +1297,7 @@
         <v>44836</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J8">
         <v>0.27021836486859202</v>
@@ -1293,7 +1306,7 @@
         <v>44836</v>
       </c>
       <c r="L8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P8" s="1"/>
       <c r="R8" s="1"/>
@@ -1316,10 +1329,10 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>10</v>
@@ -1340,7 +1353,7 @@
         <v>44854</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J9">
         <v>0.125654649037206</v>
@@ -1349,7 +1362,7 @@
         <v>44852</v>
       </c>
       <c r="L9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M9">
         <v>9</v>
@@ -1394,10 +1407,10 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>10</v>
@@ -1418,7 +1431,7 @@
         <v>44829</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10">
         <v>0.17573651879065599</v>
@@ -1427,7 +1440,7 @@
         <v>44829</v>
       </c>
       <c r="L10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1456,22 +1469,22 @@
         <v>35</v>
       </c>
       <c r="W10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X10" s="5"/>
       <c r="Y10" s="7">
         <v>44829</v>
       </c>
       <c r="Z10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>10</v>
@@ -1492,7 +1505,7 @@
         <v>44837</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11">
         <v>0.40152336927648102</v>
@@ -1501,7 +1514,7 @@
         <v>44831</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P11" s="1"/>
       <c r="R11" s="1"/>
@@ -1524,10 +1537,10 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>25</v>
@@ -1548,7 +1561,7 @@
         <v>44832</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J12">
         <v>0.30393141946306301</v>
@@ -1557,7 +1570,7 @@
         <v>44836</v>
       </c>
       <c r="L12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1590,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X12" s="6">
         <v>44840</v>
@@ -1604,10 +1617,10 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
@@ -1628,7 +1641,7 @@
         <v>44847</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J13">
         <v>9.5735609739359101E-2</v>
@@ -1637,7 +1650,7 @@
         <v>44848</v>
       </c>
       <c r="L13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M13">
         <v>15</v>
@@ -1682,10 +1695,10 @@
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>25</v>
@@ -1706,7 +1719,7 @@
         <v>44834</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J14">
         <v>0.27063232859577402</v>
@@ -1715,7 +1728,7 @@
         <v>44833</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P14" s="1"/>
       <c r="R14" s="1"/>
@@ -1738,10 +1751,10 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>10</v>
@@ -1762,7 +1775,7 @@
         <v>44852</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15">
         <v>0.13038559628954099</v>
@@ -1771,7 +1784,7 @@
         <v>44852</v>
       </c>
       <c r="L15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M15">
         <v>7</v>
@@ -1816,10 +1829,10 @@
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>10</v>
@@ -1840,7 +1853,7 @@
         <v>44836</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16">
         <v>8.6066641342581907E-2</v>
@@ -1849,7 +1862,7 @@
         <v>44835</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M16">
         <v>10</v>
@@ -1894,10 +1907,10 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>25</v>
@@ -1918,7 +1931,7 @@
         <v>44829</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J17">
         <v>0.41037681301071999</v>
@@ -1927,7 +1940,7 @@
         <v>44829</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P17" s="1"/>
       <c r="R17" s="1"/>
@@ -1950,10 +1963,10 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>10</v>
@@ -1974,7 +1987,7 @@
         <v>44855</v>
       </c>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J18">
         <v>0.109410868884129</v>
@@ -1983,7 +1996,7 @@
         <v>44856</v>
       </c>
       <c r="L18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M18">
         <v>9</v>
@@ -2028,10 +2041,10 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>10</v>
@@ -2052,7 +2065,7 @@
         <v>44854</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J19">
         <v>0.281160826740954</v>
@@ -2061,7 +2074,7 @@
         <v>44850</v>
       </c>
       <c r="L19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P19" s="1"/>
       <c r="R19" s="1"/>
@@ -2082,15 +2095,15 @@
         <v>38</v>
       </c>
       <c r="AA19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>10</v>
@@ -2111,7 +2124,7 @@
         <v>44832</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J20">
         <v>0.195840533276086</v>
@@ -2120,7 +2133,7 @@
         <v>44832</v>
       </c>
       <c r="L20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M20">
         <v>2</v>
@@ -2151,7 +2164,7 @@
         <v>24</v>
       </c>
       <c r="W20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X20" s="6">
         <v>44833</v>
@@ -2160,7 +2173,7 @@
         <v>44833</v>
       </c>
       <c r="Z20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:27">
@@ -2191,10 +2204,17 @@
       <c r="I21" t="s">
         <v>26</v>
       </c>
-      <c r="K21" s="1"/>
+      <c r="J21">
+        <v>0.53069065503624602</v>
+      </c>
+      <c r="K21" s="14">
+        <v>44831</v>
+      </c>
       <c r="L21" t="s">
         <v>11</v>
       </c>
+      <c r="P21" s="14"/>
+      <c r="R21" s="14"/>
       <c r="T21" s="8">
         <v>44846</v>
       </c>
@@ -2204,6 +2224,10 @@
       <c r="V21">
         <v>17</v>
       </c>
+      <c r="W21" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X21" s="15"/>
       <c r="Z21" t="s">
         <v>38</v>
       </c>
@@ -2236,10 +2260,17 @@
       <c r="I22" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="1"/>
+      <c r="J22">
+        <v>0.23943967503080099</v>
+      </c>
+      <c r="K22" s="14">
+        <v>44834</v>
+      </c>
       <c r="L22" t="s">
         <v>26</v>
       </c>
+      <c r="P22" s="14"/>
+      <c r="R22" s="14"/>
       <c r="T22" s="8">
         <v>44843</v>
       </c>
@@ -2249,11 +2280,15 @@
       <c r="V22">
         <v>20</v>
       </c>
+      <c r="W22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X22" s="15"/>
       <c r="Y22" s="7">
         <v>44841</v>
       </c>
       <c r="Z22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:27">
@@ -2284,10 +2319,17 @@
       <c r="I23" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="1"/>
+      <c r="J23">
+        <v>0.50641638618283402</v>
+      </c>
+      <c r="K23" s="14">
+        <v>44856</v>
+      </c>
       <c r="L23" t="s">
         <v>17</v>
       </c>
+      <c r="P23" s="14"/>
+      <c r="R23" s="14"/>
       <c r="T23" s="8">
         <v>44863</v>
       </c>
@@ -2297,6 +2339,10 @@
       <c r="V23">
         <v>0</v>
       </c>
+      <c r="W23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X23" s="15"/>
       <c r="Z23" t="s">
         <v>38</v>
       </c>
@@ -2329,10 +2375,17 @@
       <c r="I24" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="1"/>
+      <c r="J24">
+        <v>0.42815665909004103</v>
+      </c>
+      <c r="K24" s="14">
+        <v>44840</v>
+      </c>
       <c r="L24" t="s">
         <v>12</v>
       </c>
+      <c r="P24" s="14"/>
+      <c r="R24" s="14"/>
       <c r="T24" s="8">
         <v>44847</v>
       </c>
@@ -2342,11 +2395,17 @@
       <c r="V24">
         <v>16</v>
       </c>
+      <c r="W24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X24" s="16">
+        <v>44836</v>
+      </c>
       <c r="Y24" s="7">
-        <v>44834</v>
+        <v>44838</v>
       </c>
       <c r="Z24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:27">
@@ -2377,10 +2436,17 @@
       <c r="I25" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="1"/>
+      <c r="J25">
+        <v>0.38878180191077299</v>
+      </c>
+      <c r="K25" s="14">
+        <v>44832</v>
+      </c>
       <c r="L25" t="s">
         <v>12</v>
       </c>
+      <c r="P25" s="14"/>
+      <c r="R25" s="14"/>
       <c r="T25" s="8">
         <v>44842</v>
       </c>
@@ -2390,9 +2456,11 @@
       <c r="V25">
         <v>21</v>
       </c>
-      <c r="Y25" s="7">
-        <v>44842</v>
-      </c>
+      <c r="W25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X25" s="15"/>
+      <c r="Y25" s="7"/>
       <c r="Z25" t="s">
         <v>38</v>
       </c>
@@ -2425,13 +2493,32 @@
       <c r="I26" t="s">
         <v>11</v>
       </c>
-      <c r="K26" s="1"/>
+      <c r="J26">
+        <v>0.13037669001465699</v>
+      </c>
+      <c r="K26" s="14">
+        <v>44830</v>
+      </c>
       <c r="L26" t="s">
         <v>12</v>
       </c>
       <c r="M26">
         <v>0</v>
       </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26" s="14"/>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26" s="14"/>
+      <c r="S26">
+        <v>0</v>
+      </c>
       <c r="T26" s="8">
         <v>44863</v>
       </c>
@@ -2440,6 +2527,13 @@
       </c>
       <c r="V26">
         <v>0</v>
+      </c>
+      <c r="W26" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X26" s="15"/>
+      <c r="Y26" s="7">
+        <v>44860</v>
       </c>
       <c r="Z26" t="s">
         <v>37</v>
@@ -2473,13 +2567,32 @@
       <c r="I27" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="1"/>
+      <c r="J27">
+        <v>0.11186659463165</v>
+      </c>
+      <c r="K27" s="14">
+        <v>44839</v>
+      </c>
       <c r="L27" t="s">
         <v>12</v>
       </c>
       <c r="M27">
         <v>0</v>
       </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" s="14"/>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27" s="14"/>
+      <c r="S27">
+        <v>0</v>
+      </c>
       <c r="T27" s="8">
         <v>44863</v>
       </c>
@@ -2489,8 +2602,12 @@
       <c r="V27">
         <v>0</v>
       </c>
+      <c r="W27" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X27" s="15"/>
       <c r="Z27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:27">
@@ -2521,13 +2638,32 @@
       <c r="I28" t="s">
         <v>12</v>
       </c>
-      <c r="K28" s="1"/>
+      <c r="J28">
+        <v>0.15029678348968101</v>
+      </c>
+      <c r="K28" s="14">
+        <v>44846</v>
+      </c>
       <c r="L28" t="s">
         <v>12</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+      <c r="P28" s="14"/>
+      <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28" s="14"/>
+      <c r="S28">
+        <v>0</v>
+      </c>
       <c r="T28" s="8">
         <v>44863</v>
       </c>
@@ -2537,8 +2673,12 @@
       <c r="V28">
         <v>0</v>
       </c>
+      <c r="W28" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X28" s="15"/>
       <c r="Z28" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:27">
@@ -2569,10 +2709,17 @@
       <c r="I29" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="1"/>
+      <c r="J29">
+        <v>0.32213495842691198</v>
+      </c>
+      <c r="K29" s="14">
+        <v>44850</v>
+      </c>
       <c r="L29" t="s">
         <v>17</v>
       </c>
+      <c r="P29" s="14"/>
+      <c r="R29" s="14"/>
       <c r="T29" s="8">
         <v>44863</v>
       </c>
@@ -2582,11 +2729,17 @@
       <c r="V29">
         <v>0</v>
       </c>
+      <c r="W29" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X29" s="16">
+        <v>44852</v>
+      </c>
       <c r="Y29" s="7">
         <v>44851</v>
       </c>
       <c r="Z29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -2617,10 +2770,17 @@
       <c r="I30" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="1"/>
+      <c r="J30">
+        <v>0.30930929468688401</v>
+      </c>
+      <c r="K30" s="14">
+        <v>44836</v>
+      </c>
       <c r="L30" t="s">
         <v>12</v>
       </c>
+      <c r="P30" s="14"/>
+      <c r="R30" s="14"/>
       <c r="T30" s="8">
         <v>45594</v>
       </c>
@@ -2630,6 +2790,10 @@
       <c r="V30">
         <v>0</v>
       </c>
+      <c r="W30" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X30" s="15"/>
       <c r="Z30" t="s">
         <v>38</v>
       </c>
@@ -2662,10 +2826,17 @@
       <c r="I31" t="s">
         <v>26</v>
       </c>
-      <c r="K31" s="1"/>
+      <c r="J31">
+        <v>0.38186904906075603</v>
+      </c>
+      <c r="K31" s="14">
+        <v>44836</v>
+      </c>
       <c r="L31" t="s">
         <v>16</v>
       </c>
+      <c r="P31" s="14"/>
+      <c r="R31" s="14"/>
       <c r="T31" s="8">
         <v>44858</v>
       </c>
@@ -2675,11 +2846,17 @@
       <c r="V31">
         <v>4</v>
       </c>
+      <c r="W31" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X31" s="16">
+        <v>44852</v>
+      </c>
       <c r="Y31" s="7">
         <v>44852</v>
       </c>
       <c r="Z31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:27">
@@ -2710,10 +2887,17 @@
       <c r="I32" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="1"/>
+      <c r="J32">
+        <v>0.28666881052452903</v>
+      </c>
+      <c r="K32" s="14">
+        <v>44833</v>
+      </c>
       <c r="L32" t="s">
         <v>12</v>
       </c>
+      <c r="P32" s="14"/>
+      <c r="R32" s="14"/>
       <c r="T32" s="8">
         <v>44863</v>
       </c>
@@ -2723,8 +2907,12 @@
       <c r="V32">
         <v>0</v>
       </c>
+      <c r="W32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X32" s="15"/>
       <c r="Z32" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:26">
@@ -2755,13 +2943,36 @@
       <c r="I33" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="J33">
+        <v>5.6063339719054597E-2</v>
+      </c>
+      <c r="K33" s="14">
+        <v>44846</v>
+      </c>
       <c r="L33" t="s">
         <v>12</v>
       </c>
       <c r="M33">
         <v>13</v>
       </c>
+      <c r="N33">
+        <v>13</v>
+      </c>
+      <c r="O33">
+        <v>12</v>
+      </c>
+      <c r="P33" s="14">
+        <v>44836</v>
+      </c>
+      <c r="Q33">
+        <v>13</v>
+      </c>
+      <c r="R33" s="14">
+        <v>44836</v>
+      </c>
+      <c r="S33">
+        <v>13</v>
+      </c>
       <c r="T33" s="8">
         <v>44863</v>
       </c>
@@ -2771,8 +2982,12 @@
       <c r="V33">
         <v>0</v>
       </c>
+      <c r="W33" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X33" s="16"/>
       <c r="Y33" s="7">
-        <v>44837</v>
+        <v>44836</v>
       </c>
       <c r="Z33" t="s">
         <v>45</v>
@@ -2806,10 +3021,17 @@
       <c r="I34" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="1"/>
+      <c r="J34">
+        <v>0.235434426266942</v>
+      </c>
+      <c r="K34" s="14">
+        <v>44850</v>
+      </c>
       <c r="L34" t="s">
         <v>12</v>
       </c>
+      <c r="P34" s="14"/>
+      <c r="R34" s="14"/>
       <c r="T34" s="8">
         <v>44863</v>
       </c>
@@ -2819,8 +3041,12 @@
       <c r="V34">
         <v>0</v>
       </c>
+      <c r="W34" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X34" s="15"/>
       <c r="Z34" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -2851,13 +3077,36 @@
       <c r="I35" t="s">
         <v>11</v>
       </c>
-      <c r="K35" s="1"/>
+      <c r="J35">
+        <v>0.15193145632178801</v>
+      </c>
+      <c r="K35" s="14">
+        <v>44841</v>
+      </c>
       <c r="L35" t="s">
         <v>17</v>
       </c>
       <c r="M35">
         <v>1</v>
       </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" s="14">
+        <v>44841</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+      <c r="R35" s="14">
+        <v>44841</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
       <c r="T35" s="8">
         <v>44857</v>
       </c>
@@ -2867,8 +3116,12 @@
       <c r="V35">
         <v>13</v>
       </c>
+      <c r="W35" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X35" s="16"/>
       <c r="Y35" s="7">
-        <v>44842</v>
+        <v>44841</v>
       </c>
       <c r="Z35" t="s">
         <v>45</v>
@@ -2902,10 +3155,17 @@
       <c r="I36" t="s">
         <v>12</v>
       </c>
-      <c r="K36" s="1"/>
+      <c r="J36">
+        <v>0.21227982194238301</v>
+      </c>
+      <c r="K36" s="14">
+        <v>44836</v>
+      </c>
       <c r="L36" t="s">
         <v>17</v>
       </c>
+      <c r="P36" s="14"/>
+      <c r="R36" s="14"/>
       <c r="T36" s="8">
         <v>44842</v>
       </c>
@@ -2915,11 +3175,17 @@
       <c r="V36">
         <v>21</v>
       </c>
+      <c r="W36" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="X36" s="16">
+        <v>44839</v>
+      </c>
       <c r="Y36" s="7">
-        <v>44838</v>
+        <v>44839</v>
       </c>
       <c r="Z36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -2950,13 +3216,32 @@
       <c r="I37" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="1"/>
+      <c r="J37">
+        <v>0.18871150616494201</v>
+      </c>
+      <c r="K37" s="14">
+        <v>44832</v>
+      </c>
       <c r="L37" t="s">
         <v>11</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37" s="14"/>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37" s="14"/>
+      <c r="S37">
+        <v>0</v>
+      </c>
       <c r="T37" s="8">
         <v>44863</v>
       </c>
@@ -2966,8 +3251,12 @@
       <c r="V37">
         <v>0</v>
       </c>
+      <c r="W37" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X37" s="15"/>
       <c r="Z37" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -2998,10 +3287,17 @@
       <c r="I38" t="s">
         <v>16</v>
       </c>
-      <c r="K38" s="1"/>
+      <c r="J38">
+        <v>0.26198465701624402</v>
+      </c>
+      <c r="K38" s="14">
+        <v>44832</v>
+      </c>
       <c r="L38" t="s">
         <v>12</v>
       </c>
+      <c r="P38" s="14"/>
+      <c r="R38" s="14"/>
       <c r="T38" s="8">
         <v>44863</v>
       </c>
@@ -3011,8 +3307,12 @@
       <c r="V38">
         <v>0</v>
       </c>
+      <c r="W38" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X38" s="15"/>
       <c r="Z38" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated encounter summaries and script
</commit_message>
<xml_diff>
--- a/data/encounters/suspected_mortality_updated.xlsx
+++ b/data/encounters/suspected_mortality_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcusMichelangeli\GIT projects\Git_repo\drugged_lakes_griffith_repo\drugged_lakes\data\encounters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F6C519-D202-4792-94F7-24BC5ED33853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2912C2-DDD7-4396-B33D-36A61753CCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="115">
   <si>
     <t>individual_ID</t>
   </si>
@@ -293,13 +293,88 @@
   </si>
   <si>
     <t>mortality?</t>
+  </si>
+  <si>
+    <t>cow paradise</t>
+  </si>
+  <si>
+    <t>F59817</t>
+  </si>
+  <si>
+    <t>F59819</t>
+  </si>
+  <si>
+    <t>F59820</t>
+  </si>
+  <si>
+    <t>F59826</t>
+  </si>
+  <si>
+    <t>F59828</t>
+  </si>
+  <si>
+    <t>F59831</t>
+  </si>
+  <si>
+    <t>F59847</t>
+  </si>
+  <si>
+    <t>F59849</t>
+  </si>
+  <si>
+    <t>F59852</t>
+  </si>
+  <si>
+    <t>F59853</t>
+  </si>
+  <si>
+    <t>F59873</t>
+  </si>
+  <si>
+    <t>F59878</t>
+  </si>
+  <si>
+    <t>F59896</t>
+  </si>
+  <si>
+    <t>F59895</t>
+  </si>
+  <si>
+    <t>F59894</t>
+  </si>
+  <si>
+    <t>F59898</t>
+  </si>
+  <si>
+    <t>F59897</t>
+  </si>
+  <si>
+    <t>Very poor tracking. Maybe dead on 13/10/2022. Remove due to poor tracking.</t>
+  </si>
+  <si>
+    <t>Maybe dead on 27/10/2022</t>
+  </si>
+  <si>
+    <t>Maybe dead on 21/10/2022</t>
+  </si>
+  <si>
+    <t>Unclear.</t>
+  </si>
+  <si>
+    <t>Poor tracking. Remove</t>
+  </si>
+  <si>
+    <t>Maybe dead on 20/10/2022. Movement changes dramatically</t>
+  </si>
+  <si>
+    <t>poor_tracking_remove</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -370,8 +445,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +463,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -412,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -430,6 +517,9 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,16 +816,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA38"/>
+  <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A11" sqref="A11:XFD11"/>
+      <selection pane="topRight" activeCell="Z51" sqref="Z51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.7109375" customWidth="1"/>
@@ -2915,7 +3006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:26">
+    <row r="33" spans="1:27">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -2993,7 +3084,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:26">
+    <row r="34" spans="1:27">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3049,7 +3140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:26">
+    <row r="35" spans="1:27">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -3127,7 +3218,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:26">
+    <row r="36" spans="1:27">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -3188,7 +3279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:26">
+    <row r="37" spans="1:27">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -3259,7 +3350,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:26">
+    <row r="38" spans="1:27">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -3313,6 +3404,814 @@
       <c r="X38" s="15"/>
       <c r="Z38" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39" s="14">
+        <v>44849</v>
+      </c>
+      <c r="I39" t="s">
+        <v>103</v>
+      </c>
+      <c r="J39">
+        <v>0.32032749014503797</v>
+      </c>
+      <c r="K39" s="14">
+        <v>44849</v>
+      </c>
+      <c r="L39" t="s">
+        <v>105</v>
+      </c>
+      <c r="P39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="T39" s="18">
+        <v>44864</v>
+      </c>
+      <c r="U39">
+        <v>12</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+      <c r="W39" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X39" s="15"/>
+      <c r="Y39" s="7">
+        <v>44854</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA39" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27">
+      <c r="A40" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40">
+        <v>65</v>
+      </c>
+      <c r="G40">
+        <v>43</v>
+      </c>
+      <c r="H40" s="14">
+        <v>44836</v>
+      </c>
+      <c r="I40" t="s">
+        <v>104</v>
+      </c>
+      <c r="J40">
+        <v>0.26104063548393502</v>
+      </c>
+      <c r="K40" s="14">
+        <v>44845</v>
+      </c>
+      <c r="L40" t="s">
+        <v>105</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40" s="14">
+        <v>44836</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40" s="14"/>
+      <c r="S40">
+        <v>0</v>
+      </c>
+      <c r="T40" s="18">
+        <v>44854</v>
+      </c>
+      <c r="U40">
+        <v>21</v>
+      </c>
+      <c r="V40">
+        <v>11</v>
+      </c>
+      <c r="W40" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X40" s="15"/>
+      <c r="Z40" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA40" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27">
+      <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41">
+        <v>45</v>
+      </c>
+      <c r="G41">
+        <v>28</v>
+      </c>
+      <c r="H41" s="14">
+        <v>44845</v>
+      </c>
+      <c r="I41" t="s">
+        <v>103</v>
+      </c>
+      <c r="J41">
+        <v>0.15874153900235499</v>
+      </c>
+      <c r="K41" s="14">
+        <v>44845</v>
+      </c>
+      <c r="L41" t="s">
+        <v>105</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41" s="14">
+        <v>44845</v>
+      </c>
+      <c r="Q41">
+        <v>1</v>
+      </c>
+      <c r="R41" s="14"/>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41" s="18">
+        <v>44864</v>
+      </c>
+      <c r="U41">
+        <v>14</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+      <c r="W41" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X41" s="15"/>
+      <c r="Z41" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA41" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27">
+      <c r="A42" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="15"/>
+      <c r="F42">
+        <v>104</v>
+      </c>
+      <c r="G42">
+        <v>58</v>
+      </c>
+      <c r="H42" s="14">
+        <v>44831</v>
+      </c>
+      <c r="I42" t="s">
+        <v>105</v>
+      </c>
+      <c r="J42">
+        <v>0.227024932571322</v>
+      </c>
+      <c r="K42" s="14">
+        <v>44847</v>
+      </c>
+      <c r="L42" t="s">
+        <v>105</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>0</v>
+      </c>
+      <c r="P42" s="14">
+        <v>44831</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="R42" s="14"/>
+      <c r="S42">
+        <v>0</v>
+      </c>
+      <c r="T42" s="18">
+        <v>44864</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <v>2</v>
+      </c>
+      <c r="W42" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="7">
+        <v>44854</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27">
+      <c r="A43" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="16">
+        <v>44855</v>
+      </c>
+      <c r="F43">
+        <v>516</v>
+      </c>
+      <c r="G43">
+        <v>256</v>
+      </c>
+      <c r="H43" s="14">
+        <v>44853</v>
+      </c>
+      <c r="I43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43">
+        <v>0.22709957940220299</v>
+      </c>
+      <c r="K43" s="14">
+        <v>44847</v>
+      </c>
+      <c r="L43" t="s">
+        <v>105</v>
+      </c>
+      <c r="M43">
+        <v>4</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+      <c r="P43" s="14">
+        <v>44852</v>
+      </c>
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43" s="14">
+        <v>44852</v>
+      </c>
+      <c r="S43">
+        <v>2</v>
+      </c>
+      <c r="T43" s="18">
+        <v>44861</v>
+      </c>
+      <c r="U43">
+        <v>20</v>
+      </c>
+      <c r="V43">
+        <v>4</v>
+      </c>
+      <c r="W43" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="7">
+        <v>44853</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27">
+      <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44">
+        <v>28</v>
+      </c>
+      <c r="G44">
+        <v>9</v>
+      </c>
+      <c r="H44" s="14">
+        <v>44836</v>
+      </c>
+      <c r="I44" t="s">
+        <v>105</v>
+      </c>
+      <c r="J44">
+        <v>0.30388211928473202</v>
+      </c>
+      <c r="K44" s="14">
+        <v>44847</v>
+      </c>
+      <c r="L44" t="s">
+        <v>105</v>
+      </c>
+      <c r="P44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="T44" s="18">
+        <v>44864</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="W44" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X44" s="15"/>
+      <c r="Y44" s="7"/>
+      <c r="Z44" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA44" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27">
+      <c r="A45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="16">
+        <v>44845</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" s="14">
+        <v>44831</v>
+      </c>
+      <c r="I45" t="s">
+        <v>105</v>
+      </c>
+      <c r="J45">
+        <v>0.58768965719311805</v>
+      </c>
+      <c r="K45" s="14">
+        <v>44834</v>
+      </c>
+      <c r="L45" t="s">
+        <v>105</v>
+      </c>
+      <c r="P45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="T45" s="18">
+        <v>44864</v>
+      </c>
+      <c r="U45">
+        <v>14</v>
+      </c>
+      <c r="V45">
+        <v>16</v>
+      </c>
+      <c r="W45" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X45" s="16">
+        <v>44845</v>
+      </c>
+      <c r="Y45" s="7">
+        <v>44844</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46">
+        <v>8</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46" s="14">
+        <v>44844</v>
+      </c>
+      <c r="I46" t="s">
+        <v>103</v>
+      </c>
+      <c r="J46">
+        <v>0.318841744262777</v>
+      </c>
+      <c r="K46" s="14">
+        <v>44834</v>
+      </c>
+      <c r="L46" t="s">
+        <v>105</v>
+      </c>
+      <c r="P46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="T46" s="18">
+        <v>44846</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>19</v>
+      </c>
+      <c r="W46" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X46" s="15"/>
+      <c r="Y46" s="7">
+        <v>44844</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E47" s="16">
+        <v>44854</v>
+      </c>
+      <c r="F47">
+        <v>35</v>
+      </c>
+      <c r="G47">
+        <v>27</v>
+      </c>
+      <c r="H47" s="14">
+        <v>44833</v>
+      </c>
+      <c r="I47" t="s">
+        <v>104</v>
+      </c>
+      <c r="J47">
+        <v>0.36869846370220599</v>
+      </c>
+      <c r="K47" s="14">
+        <v>44833</v>
+      </c>
+      <c r="L47" t="s">
+        <v>105</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47" s="14">
+        <v>44833</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47" s="14"/>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47" s="18">
+        <v>44860</v>
+      </c>
+      <c r="U47">
+        <v>9</v>
+      </c>
+      <c r="V47">
+        <v>5</v>
+      </c>
+      <c r="W47" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X47" s="16">
+        <v>44854</v>
+      </c>
+      <c r="Y47" s="7">
+        <v>44854</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA47" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E48" s="16">
+        <v>44836</v>
+      </c>
+      <c r="F48">
+        <v>14</v>
+      </c>
+      <c r="G48">
+        <v>14</v>
+      </c>
+      <c r="H48" s="14">
+        <v>44833</v>
+      </c>
+      <c r="I48" t="s">
+        <v>103</v>
+      </c>
+      <c r="J48">
+        <v>0.26264801756020301</v>
+      </c>
+      <c r="K48" s="14">
+        <v>44833</v>
+      </c>
+      <c r="L48" t="s">
+        <v>105</v>
+      </c>
+      <c r="P48" s="14"/>
+      <c r="R48" s="14"/>
+      <c r="T48" s="18">
+        <v>44851</v>
+      </c>
+      <c r="U48">
+        <v>9</v>
+      </c>
+      <c r="V48">
+        <v>20</v>
+      </c>
+      <c r="W48" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X48" s="16">
+        <v>44836</v>
+      </c>
+      <c r="Y48" s="7">
+        <v>44836</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49" s="14">
+        <v>44831</v>
+      </c>
+      <c r="I49" t="s">
+        <v>105</v>
+      </c>
+      <c r="J49">
+        <v>0.49282965696073899</v>
+      </c>
+      <c r="K49" s="14">
+        <v>44832</v>
+      </c>
+      <c r="L49" t="s">
+        <v>105</v>
+      </c>
+      <c r="P49" s="14"/>
+      <c r="R49" s="14"/>
+      <c r="T49" s="18">
+        <v>44834</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>31</v>
+      </c>
+      <c r="W49" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="X49" s="15"/>
+      <c r="Z49" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA49" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="16">
+        <v>44845</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" s="14">
+        <v>44842</v>
+      </c>
+      <c r="I50" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50">
+        <v>0.44785087225759201</v>
+      </c>
+      <c r="K50" s="14">
+        <v>44842</v>
+      </c>
+      <c r="L50" t="s">
+        <v>105</v>
+      </c>
+      <c r="P50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="T50" s="18">
+        <v>44853</v>
+      </c>
+      <c r="U50">
+        <v>13</v>
+      </c>
+      <c r="V50">
+        <v>11</v>
+      </c>
+      <c r="W50" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="X50" s="16">
+        <v>44845</v>
+      </c>
+      <c r="Y50" s="7">
+        <v>44844</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>